<commit_message>
apps done til spinnerview
</commit_message>
<xml_diff>
--- a/AndroidProgramList.xlsx
+++ b/AndroidProgramList.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rushik\sem6\Android\AndroidProjects\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Android Program" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Android Program</t>
   </si>
@@ -119,7 +114,28 @@
     <t>RadioButton(Traffic Signal App)</t>
   </si>
   <si>
-    <t>Handling View Events</t>
+    <t>progressBar View</t>
+  </si>
+  <si>
+    <t>Basic View 2</t>
+  </si>
+  <si>
+    <t>AutoCompleteTextView</t>
+  </si>
+  <si>
+    <t>UsingPickerView</t>
+  </si>
+  <si>
+    <t>ListView</t>
+  </si>
+  <si>
+    <t>SpinnerView</t>
+  </si>
+  <si>
+    <t>DatePicker</t>
+  </si>
+  <si>
+    <t>TimePicker</t>
   </si>
 </sst>
 </file>
@@ -310,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,7 +361,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +874,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
@@ -869,26 +885,79 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D28">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3:D35">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$D$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
contextmenu app done, grid view app done
</commit_message>
<xml_diff>
--- a/AndroidProgramList.xlsx
+++ b/AndroidProgramList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Android Program</t>
   </si>
@@ -122,9 +122,6 @@
     <t>progressBar View</t>
   </si>
   <si>
-    <t>Basic View 2</t>
-  </si>
-  <si>
     <t>AutoCompleteTextView</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>External Storage</t>
+  </si>
+  <si>
+    <t>Basic View 2(ProgressBar)</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -486,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +891,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -849,7 +899,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -857,7 +907,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -865,7 +915,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" t="s">
         <v>2</v>
@@ -873,7 +923,7 @@
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -881,7 +931,7 @@
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>2</v>
@@ -889,7 +939,7 @@
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
@@ -897,31 +947,46 @@
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D35">
+  <conditionalFormatting sqref="D3:D38 D40:D41">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$D$3</formula>
     </cfRule>

</xml_diff>

<commit_message>
adnrodi progrma list add tutotial 3
</commit_message>
<xml_diff>
--- a/AndroidProgramList.xlsx
+++ b/AndroidProgramList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>Android Program</t>
   </si>
@@ -156,6 +156,48 @@
   </si>
   <si>
     <t>Basic View 2(ProgressBar)</t>
+  </si>
+  <si>
+    <t>SqliteApp</t>
+  </si>
+  <si>
+    <t>AnimationApp</t>
+  </si>
+  <si>
+    <t>ContentProvider</t>
+  </si>
+  <si>
+    <t>Custom Content Provider</t>
+  </si>
+  <si>
+    <t>Location Base Service Pg 371</t>
+  </si>
+  <si>
+    <t>Geo Coding and Reverse Geo Coding Pg 337</t>
+  </si>
+  <si>
+    <t>Navigating Map For Specific Locatoin</t>
+  </si>
+  <si>
+    <t>Perform</t>
+  </si>
+  <si>
+    <t>Networking Api</t>
+  </si>
+  <si>
+    <t>Telephony</t>
+  </si>
+  <si>
+    <t>BlinkLights</t>
+  </si>
+  <si>
+    <t>Mysql-Json</t>
+  </si>
+  <si>
+    <t>Tutorial 3</t>
+  </si>
+  <si>
+    <t>Tutorial 2</t>
   </si>
 </sst>
 </file>
@@ -171,12 +213,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -191,15 +239,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -536,17 +646,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -804,56 +914,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>7</v>
+      <c r="C22" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -861,53 +943,62 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>30</v>
       </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
-        <v>32</v>
-      </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -915,78 +1006,228 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>34</v>
       </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>35</v>
       </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>38</v>
       </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>39</v>
       </c>
-      <c r="D37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="D38" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>43484</v>
+      </c>
+      <c r="C45" t="s">
         <v>41</v>
       </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>43486</v>
+      </c>
+      <c r="C46" t="s">
         <v>42</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>43488</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>43493</v>
+      </c>
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>43496</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>43497</v>
+      </c>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>43498</v>
+      </c>
+      <c r="C52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>43503</v>
+      </c>
+      <c r="C54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
+        <v>43505</v>
+      </c>
+      <c r="C55" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="2">
+        <v>43509</v>
+      </c>
+      <c r="C56" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>43511</v>
+      </c>
+      <c r="C57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D38 D40:D41">
+  <conditionalFormatting sqref="D45:D57 D3:D20 D24:D41">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$D$3</formula>
     </cfRule>

</xml_diff>